<commit_message>
Download file process handled.
It downloads the file after generating it. There is only, Run button deactivation left.
</commit_message>
<xml_diff>
--- a/App/Files/TestResult_240807_1.xlsx
+++ b/App/Files/TestResult_240807_1.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>